<commit_message>
modify sprint form and add a need for backend
</commit_message>
<xml_diff>
--- a/doc/迭代开发_早睡早起.xlsx
+++ b/doc/迭代开发_早睡早起.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="2" r:id="rId1"/>
@@ -1436,14 +1436,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.734375" customWidth="1"/>
-    <col min="2" max="2" width="24.734375" customWidth="1"/>
-    <col min="3" max="3" width="78.62890625" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -1534,17 +1534,17 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.62890625" customWidth="1"/>
-    <col min="2" max="2" width="14.734375" customWidth="1"/>
-    <col min="3" max="3" width="38.20703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.26171875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.47265625" customWidth="1"/>
+    <col min="5" max="5" width="48.21875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>1</f>
         <v>1</v>
@@ -1583,7 +1583,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1602,7 +1602,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="1">A3+1</f>
         <v>3</v>
@@ -1621,7 +1621,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1640,7 +1640,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1659,7 +1659,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1678,7 +1678,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1697,7 +1697,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1713,7 +1713,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1732,7 +1732,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1751,7 +1751,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1770,7 +1770,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1789,7 +1789,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1808,7 +1808,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1827,7 +1827,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1846,7 +1846,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1865,7 +1865,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1884,7 +1884,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1903,7 +1903,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1922,7 +1922,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1941,7 +1941,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1960,7 +1960,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1979,7 +1979,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1998,7 +1998,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -2017,7 +2017,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -2036,7 +2036,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -2055,7 +2055,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -2074,7 +2074,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -2093,7 +2093,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -2112,7 +2112,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -2131,7 +2131,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -2150,7 +2150,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -2169,7 +2169,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -2188,7 +2188,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="42.3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2204,7 +2204,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2223,7 +2223,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2242,7 +2242,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -2258,7 +2258,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2277,7 +2277,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2296,7 +2296,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2312,7 +2312,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2328,7 +2328,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2344,7 +2344,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2360,7 +2360,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2376,7 +2376,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2392,7 +2392,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2408,7 +2408,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2424,7 +2424,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2440,7 +2440,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2456,7 +2456,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2472,7 +2472,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2488,7 +2488,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2504,7 +2504,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2520,7 +2520,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2536,7 +2536,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2555,7 +2555,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2574,7 +2574,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2593,7 +2593,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2612,7 +2612,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -2631,7 +2631,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2650,7 +2650,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2666,7 +2666,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2685,7 +2685,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="42.3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2704,7 +2704,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2723,7 +2723,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -2742,7 +2742,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -2761,7 +2761,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ref="A68:A87" si="3">A67+1</f>
         <v>67</v>
@@ -2780,7 +2780,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="3"/>
         <v>68</v>
@@ -2799,7 +2799,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="3"/>
         <v>69</v>
@@ -2818,7 +2818,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="3"/>
         <v>70</v>
@@ -2837,7 +2837,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="3"/>
         <v>71</v>
@@ -2856,91 +2856,91 @@
         <v>245</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="3"/>
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="3"/>
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="3"/>
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -2961,17 +2961,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.734375" customWidth="1"/>
-    <col min="2" max="2" width="18.62890625" customWidth="1"/>
-    <col min="3" max="3" width="14.62890625" customWidth="1"/>
-    <col min="4" max="4" width="19.26171875" customWidth="1"/>
-    <col min="5" max="5" width="20.47265625" customWidth="1"/>
-    <col min="6" max="6" width="19.89453125" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3008,7 +3008,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="42.3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3025,7 +3025,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="56.4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3059,7 +3059,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="42.3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3076,7 +3076,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="126.9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="129.6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3093,7 +3093,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="56.4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3110,7 +3110,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="42.3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3127,7 +3127,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="112.8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="115.2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -3152,7 +3152,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3160,7 +3160,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3168,7 +3168,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3176,7 +3176,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3184,7 +3184,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -3192,7 +3192,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -3200,7 +3200,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3208,7 +3208,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3216,7 +3216,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3224,7 +3224,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -3247,17 +3247,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.734375" customWidth="1"/>
-    <col min="2" max="2" width="18.62890625" customWidth="1"/>
-    <col min="3" max="3" width="14.62890625" customWidth="1"/>
-    <col min="4" max="4" width="19.26171875" customWidth="1"/>
-    <col min="5" max="5" width="20.47265625" customWidth="1"/>
-    <col min="6" max="6" width="19.89453125" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>INDEX('Product Backlog'!A:A, MATCH(B2,'Product Backlog'!C:C, 0))</f>
         <v>1</v>
@@ -3298,7 +3298,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>INDEX('Product Backlog'!A:A, MATCH(B3,'Product Backlog'!C:C, 0))</f>
         <v>2</v>
@@ -3319,7 +3319,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>INDEX('Product Backlog'!A:A, MATCH(B4,'Product Backlog'!C:C, 0))</f>
         <v>3</v>
@@ -3340,7 +3340,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>INDEX('Product Backlog'!A:A, MATCH(B5,'Product Backlog'!C:C, 0))</f>
         <v>10</v>
@@ -3361,7 +3361,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>INDEX('Product Backlog'!A:A, MATCH(B6,'Product Backlog'!C:C, 0))</f>
         <v>5</v>
@@ -3382,7 +3382,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>INDEX('Product Backlog'!A:A, MATCH(B7,'Product Backlog'!C:C, 0))</f>
         <v>6</v>
@@ -3403,7 +3403,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3411,7 +3411,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3419,7 +3419,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3427,7 +3427,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -3435,7 +3435,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -3443,7 +3443,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3451,7 +3451,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3459,7 +3459,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3467,7 +3467,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -3475,7 +3475,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -3483,7 +3483,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3491,7 +3491,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3499,7 +3499,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3507,7 +3507,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -3526,21 +3526,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.3671875" customWidth="1"/>
-    <col min="2" max="2" width="38.20703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.89453125" customWidth="1"/>
-    <col min="5" max="5" width="18.3671875" customWidth="1"/>
-    <col min="6" max="6" width="17.3671875" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>INDEX('Product Backlog'!A:A, MATCH(B2,'Product Backlog'!C:C, 0))</f>
         <v>58</v>
@@ -3579,7 +3579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>INDEX('Product Backlog'!A:A, MATCH(B3,'Product Backlog'!C:C, 0))</f>
         <v>13</v>
@@ -3598,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>INDEX('Product Backlog'!A:A, MATCH(B4,'Product Backlog'!C:C, 0))</f>
         <v>14</v>
@@ -3617,7 +3617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>INDEX('Product Backlog'!A:A, MATCH(B5,'Product Backlog'!C:C, 0))</f>
         <v>15</v>
@@ -3636,7 +3636,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>INDEX('Product Backlog'!A:A, MATCH(B6,'Product Backlog'!C:C, 0))</f>
         <v>16</v>
@@ -3649,7 +3649,7 @@
         <v>白云仁</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>INDEX('Product Backlog'!A:A, MATCH(B7,'Product Backlog'!C:C, 0))</f>
         <v>17</v>
@@ -3668,7 +3668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>INDEX('Product Backlog'!A:A, MATCH(B8,'Product Backlog'!C:C, 0))</f>
         <v>18</v>
@@ -3681,7 +3681,7 @@
         <v>白云仁</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>INDEX('Product Backlog'!A:A, MATCH(B9,'Product Backlog'!C:C, 0))</f>
         <v>19</v>
@@ -3697,7 +3697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>INDEX('Product Backlog'!A:A, MATCH(B10,'Product Backlog'!C:C, 0))</f>
         <v>20</v>
@@ -3710,7 +3710,7 @@
         <v>段清楠</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>INDEX('Product Backlog'!A:A, MATCH(B11,'Product Backlog'!C:C, 0))</f>
         <v>21</v>
@@ -3729,7 +3729,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>INDEX('Product Backlog'!A:A, MATCH(B12,'Product Backlog'!C:C, 0))</f>
         <v>22</v>
@@ -3742,7 +3742,7 @@
         <v>段清楠</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>INDEX('Product Backlog'!A:A, MATCH(B13,'Product Backlog'!C:C, 0))</f>
         <v>23</v>
@@ -3757,8 +3757,11 @@
       <c r="D13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>INDEX('Product Backlog'!A:A, MATCH(B14,'Product Backlog'!C:C, 0))</f>
         <v>24</v>
@@ -3774,7 +3777,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>INDEX('Product Backlog'!A:A, MATCH(B15,'Product Backlog'!C:C, 0))</f>
         <v>25</v>
@@ -3790,7 +3793,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>INDEX('Product Backlog'!A:A, MATCH(B16,'Product Backlog'!C:C, 0))</f>
         <v>26</v>
@@ -3805,8 +3808,11 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>INDEX('Product Backlog'!A:A, MATCH(B17,'Product Backlog'!C:C, 0))</f>
         <v>27</v>
@@ -3822,7 +3828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>INDEX('Product Backlog'!A:A, MATCH(B18,'Product Backlog'!C:C, 0))</f>
         <v>28</v>
@@ -3838,7 +3844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>INDEX('Product Backlog'!A:A, MATCH(B19,'Product Backlog'!C:C, 0))</f>
         <v>29</v>
@@ -3851,10 +3857,13 @@
         <v>侯禺凡</v>
       </c>
       <c r="D19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>INDEX('Product Backlog'!A:A, MATCH(B20,'Product Backlog'!C:C, 0))</f>
         <v>30</v>
@@ -3870,7 +3879,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>INDEX('Product Backlog'!A:A, MATCH(B21,'Product Backlog'!C:C, 0))</f>
         <v>31</v>
@@ -3886,7 +3895,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>INDEX('Product Backlog'!A:A, MATCH(B22,'Product Backlog'!C:C, 0))</f>
         <v>32</v>
@@ -3905,7 +3914,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>INDEX('Product Backlog'!A:A, MATCH(B23,'Product Backlog'!C:C, 0))</f>
         <v>33</v>
@@ -3924,7 +3933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>INDEX('Product Backlog'!A:A, MATCH(B24,'Product Backlog'!C:C, 0))</f>
         <v>55</v>
@@ -3939,8 +3948,11 @@
       <c r="D24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>INDEX('Product Backlog'!A:A, MATCH(B25,'Product Backlog'!C:C, 0))</f>
         <v>35</v>
@@ -3953,7 +3965,7 @@
         <v>白云仁</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>INDEX('Product Backlog'!A:A, MATCH(B26,'Product Backlog'!C:C, 0))</f>
         <v>36</v>
@@ -3966,7 +3978,7 @@
         <v>白云仁</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>INDEX('Product Backlog'!A:A, MATCH(B27,'Product Backlog'!C:C, 0))</f>
         <v>38</v>
@@ -3979,7 +3991,7 @@
         <v>段清楠 邵韵秋 白云仁</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>INDEX('Product Backlog'!A:A, MATCH(B28,'Product Backlog'!C:C, 0))</f>
         <v>39</v>
@@ -3995,7 +4007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>INDEX('Product Backlog'!A:A, MATCH(B29,'Product Backlog'!C:C, 0))</f>
         <v>57</v>
@@ -4011,7 +4023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>INDEX('Product Backlog'!A:A, MATCH(B30,'Product Backlog'!C:C, 0))</f>
         <v>11</v>
@@ -4027,7 +4039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>INDEX('Product Backlog'!A:A, MATCH(B31,'Product Backlog'!C:C, 0))</f>
         <v>59</v>
@@ -4042,8 +4054,11 @@
       <c r="D31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>INDEX('Product Backlog'!A:A, MATCH(B32,'Product Backlog'!C:C, 0))</f>
         <v>60</v>
@@ -4059,7 +4074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>INDEX('Product Backlog'!A:A, MATCH(B33,'Product Backlog'!C:C, 0))</f>
         <v>62</v>
@@ -4072,7 +4087,7 @@
         <v>段清楠</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>INDEX('Product Backlog'!A:A, MATCH(B34,'Product Backlog'!C:C, 0))</f>
         <v>63</v>
@@ -4084,8 +4099,14 @@
         <f>IF(VLOOKUP(B34, 'Product Backlog'!$C:$E, 2, FALSE)=0,"",VLOOKUP(B34, 'Product Backlog'!$C:$E, 2, FALSE))</f>
         <v>侯禺凡</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>INDEX('Product Backlog'!A:A, MATCH(B35,'Product Backlog'!C:C, 0))</f>
         <v>64</v>
@@ -4097,8 +4118,14 @@
         <f>IF(VLOOKUP(B35, 'Product Backlog'!$C:$E, 2, FALSE)=0,"",VLOOKUP(B35, 'Product Backlog'!$C:$E, 2, FALSE))</f>
         <v>侯禺凡</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>INDEX('Product Backlog'!A:A, MATCH(B36,'Product Backlog'!C:C, 0))</f>
         <v>65</v>
@@ -4110,8 +4137,14 @@
         <f>IF(VLOOKUP(B36, 'Product Backlog'!$C:$E, 2, FALSE)=0,"",VLOOKUP(B36, 'Product Backlog'!$C:$E, 2, FALSE))</f>
         <v>侯禺凡</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>INDEX('Product Backlog'!A:A, MATCH(B37,'Product Backlog'!C:C, 0))</f>
         <v>12</v>
@@ -4124,7 +4157,7 @@
         <v>李昊阳</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>INDEX('Product Backlog'!A:A, MATCH(B38,'Product Backlog'!C:C, 0))</f>
         <v>68</v>
@@ -4137,7 +4170,7 @@
         <v>李昊阳</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>INDEX('Product Backlog'!A:A, MATCH(B39,'Product Backlog'!C:C, 0))</f>
         <v>69</v>
@@ -4150,7 +4183,7 @@
         <v>李昊阳</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>INDEX('Product Backlog'!A:A, MATCH(B40,'Product Backlog'!C:C, 0))</f>
         <v>70</v>
@@ -4163,7 +4196,7 @@
         <v>李昊阳</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>INDEX('Product Backlog'!A:A, MATCH(B41,'Product Backlog'!C:C, 0))</f>
         <v>71</v>
@@ -4176,7 +4209,7 @@
         <v>李昊阳</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>INDEX('Product Backlog'!A:A, MATCH(B42,'Product Backlog'!C:C, 0))</f>
         <v>7</v>
@@ -4188,53 +4221,59 @@
         <f>IF(VLOOKUP(B42, 'Product Backlog'!$C:$E, 2, FALSE)=0,"",VLOOKUP(B42, 'Product Backlog'!$C:$E, 2, FALSE))</f>
         <v>侯禺凡</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="4"/>
     </row>
   </sheetData>
@@ -4252,9 +4291,9 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.1015625" defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -4288,9 +4327,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.62890625" defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>